<commit_message>
only plotting k important features
</commit_message>
<xml_diff>
--- a/python/plots_tabs/DecisionTreeRegressor_metrics.xlsx
+++ b/python/plots_tabs/DecisionTreeRegressor_metrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,21 @@
           <t>R^2</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_median</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_median</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Dir_accuracy</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +501,15 @@
       <c r="F2" t="n">
         <v>-0.04933116388098369</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.0004272416930457168</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.02066982395635263</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3446808510638298</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,6 +530,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>0.001083194070471167</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.03291191380748265</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>